<commit_message>
made plto and deviation functions
</commit_message>
<xml_diff>
--- a/data/MASTER Xenon Literature Review.xlsx
+++ b/data/MASTER Xenon Literature Review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23059859_student_uwa_edu_au/Documents/UWA/05. Year 5/Semester 1/GENG5511 MPE Engineering Research Project/Project/Research_Project/GENG5511_Thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{262D6BEE-4B49-414C-8989-11032CF05A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F734CECE-B7E6-4E4B-8629-7736254A249C}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{262D6BEE-4B49-414C-8989-11032CF05A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{926AA0DC-7035-4B31-90F4-A233872BCBFA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="6" activeTab="6" xr2:uid="{69D65117-2E76-C546-90A2-B362171284DD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{69D65117-2E76-C546-90A2-B362171284DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cell Volume " sheetId="1" r:id="rId1"/>
@@ -1464,13 +1464,28 @@
     <xf numFmtId="4" fontId="23" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1487,21 +1502,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1986,20 +1986,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F513A9-1C82-3E45-A361-2C7180831D5E}">
   <dimension ref="A1:AE373"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="63" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A212" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AC231" sqref="AC231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.08203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="7" width="17.08203125" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="13.08203125" customWidth="1"/>
+    <col min="11" max="11" width="12.08203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.9140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
     <col min="14" max="14" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.08203125" bestFit="1" customWidth="1"/>
@@ -2012,18 +2014,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
       <c r="K1" s="20" t="s">
         <v>1</v>
       </c>
@@ -2047,17 +2049,17 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="5"/>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
       <c r="K2" s="2">
         <f>6.02214076*10^23</f>
         <v>6.0221407599999999E+23</v>
@@ -2081,7 +2083,7 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="64" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="62" t="s">
@@ -2109,7 +2111,7 @@
       <c r="J3" s="62"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="68" t="s">
+      <c r="M3" s="64" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="62" t="s">
@@ -2143,7 +2145,7 @@
       <c r="Z3" s="62"/>
     </row>
     <row r="4" spans="1:26" ht="16.5">
-      <c r="A4" s="68"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
@@ -2153,10 +2155,10 @@
       <c r="F4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="63" t="s">
+      <c r="G4" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="63"/>
+      <c r="H4" s="68"/>
       <c r="I4" s="7" t="s">
         <v>17</v>
       </c>
@@ -2165,7 +2167,7 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="68"/>
+      <c r="M4" s="64"/>
       <c r="N4" s="62"/>
       <c r="O4" s="62"/>
       <c r="P4" s="62"/>
@@ -2178,12 +2180,12 @@
       <c r="S4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="63" t="s">
+      <c r="T4" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="U4" s="63"/>
-      <c r="V4" s="63"/>
-      <c r="W4" s="63"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="68"/>
+      <c r="W4" s="68"/>
       <c r="X4" s="7"/>
       <c r="Y4" s="7" t="s">
         <v>17</v>
@@ -2193,10 +2195,10 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="17" thickBot="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -2217,10 +2219,10 @@
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="70"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
       <c r="Q5" s="10" t="s">
         <v>20</v>
       </c>
@@ -2251,7 +2253,7 @@
       </c>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="69" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -2278,7 +2280,7 @@
         <f>I6^3</f>
         <v>242.97062400000002</v>
       </c>
-      <c r="N6" s="66" t="s">
+      <c r="N6" s="71" t="s">
         <v>33</v>
       </c>
       <c r="O6" s="21">
@@ -2302,7 +2304,7 @@
       </c>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="65"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="28" t="s">
         <v>31</v>
       </c>
@@ -2327,7 +2329,7 @@
         <f>I7^3</f>
         <v>236.02903199999997</v>
       </c>
-      <c r="N7" s="67"/>
+      <c r="N7" s="72"/>
       <c r="O7" s="22">
         <v>1962</v>
       </c>
@@ -2349,7 +2351,7 @@
       </c>
     </row>
     <row r="8" spans="1:26">
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="67" t="s">
         <v>36</v>
       </c>
       <c r="C8">
@@ -2373,7 +2375,7 @@
         <f t="shared" ref="J8:J26" si="2">I8^3</f>
         <v>236.60238162499996</v>
       </c>
-      <c r="N8" s="67"/>
+      <c r="N8" s="72"/>
       <c r="O8" s="22">
         <v>1962</v>
       </c>
@@ -2395,7 +2397,7 @@
       </c>
     </row>
     <row r="9" spans="1:26">
-      <c r="B9" s="61"/>
+      <c r="B9" s="67"/>
       <c r="C9">
         <v>1957</v>
       </c>
@@ -2417,7 +2419,7 @@
         <f t="shared" si="2"/>
         <v>239.02058981600004</v>
       </c>
-      <c r="N9" s="67"/>
+      <c r="N9" s="72"/>
       <c r="O9" s="22">
         <v>1962</v>
       </c>
@@ -2439,7 +2441,7 @@
       </c>
     </row>
     <row r="10" spans="1:26">
-      <c r="B10" s="61"/>
+      <c r="B10" s="67"/>
       <c r="C10">
         <v>1957</v>
       </c>
@@ -2461,7 +2463,7 @@
         <f t="shared" si="2"/>
         <v>240.17788569600003</v>
       </c>
-      <c r="N10" s="67"/>
+      <c r="N10" s="72"/>
       <c r="O10" s="22">
         <v>1962</v>
       </c>
@@ -2483,7 +2485,7 @@
       </c>
     </row>
     <row r="11" spans="1:26">
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="67" t="s">
         <v>38</v>
       </c>
       <c r="C11">
@@ -2506,7 +2508,7 @@
         <f t="shared" si="2"/>
         <v>230.53809234201302</v>
       </c>
-      <c r="N11" s="67"/>
+      <c r="N11" s="72"/>
       <c r="O11" s="22">
         <v>1962</v>
       </c>
@@ -2528,7 +2530,7 @@
       </c>
     </row>
     <row r="12" spans="1:26">
-      <c r="B12" s="61"/>
+      <c r="B12" s="67"/>
       <c r="C12">
         <v>1962</v>
       </c>
@@ -2549,7 +2551,7 @@
         <f t="shared" si="2"/>
         <v>230.54937184943202</v>
       </c>
-      <c r="N12" s="67"/>
+      <c r="N12" s="72"/>
       <c r="O12" s="22">
         <v>1962</v>
       </c>
@@ -2571,7 +2573,7 @@
       </c>
     </row>
     <row r="13" spans="1:26">
-      <c r="B13" s="61"/>
+      <c r="B13" s="67"/>
       <c r="C13">
         <v>1962</v>
       </c>
@@ -2592,7 +2594,7 @@
         <f t="shared" si="2"/>
         <v>230.62833870312502</v>
       </c>
-      <c r="N13" s="67"/>
+      <c r="N13" s="72"/>
       <c r="O13" s="22">
         <v>1962</v>
       </c>
@@ -2614,7 +2616,7 @@
       </c>
     </row>
     <row r="14" spans="1:26">
-      <c r="B14" s="61"/>
+      <c r="B14" s="67"/>
       <c r="C14">
         <v>1962</v>
       </c>
@@ -2635,7 +2637,7 @@
         <f t="shared" si="2"/>
         <v>230.79761410400002</v>
       </c>
-      <c r="N14" s="67"/>
+      <c r="N14" s="72"/>
       <c r="O14" s="22">
         <v>1962</v>
       </c>
@@ -2657,7 +2659,7 @@
       </c>
     </row>
     <row r="15" spans="1:26">
-      <c r="B15" s="61"/>
+      <c r="B15" s="67"/>
       <c r="C15">
         <v>1962</v>
       </c>
@@ -2678,7 +2680,7 @@
         <f t="shared" si="2"/>
         <v>231.068626996544</v>
       </c>
-      <c r="N15" s="67"/>
+      <c r="N15" s="72"/>
       <c r="O15" s="22">
         <v>1962</v>
       </c>
@@ -2700,7 +2702,7 @@
       </c>
     </row>
     <row r="16" spans="1:26">
-      <c r="B16" s="61"/>
+      <c r="B16" s="67"/>
       <c r="C16">
         <v>1962</v>
       </c>
@@ -2746,7 +2748,7 @@
       </c>
     </row>
     <row r="17" spans="1:26">
-      <c r="B17" s="61"/>
+      <c r="B17" s="67"/>
       <c r="C17">
         <v>1962</v>
       </c>
@@ -2789,7 +2791,7 @@
       </c>
     </row>
     <row r="18" spans="1:26">
-      <c r="B18" s="61"/>
+      <c r="B18" s="67"/>
       <c r="C18">
         <v>1962</v>
       </c>
@@ -2832,7 +2834,7 @@
       </c>
     </row>
     <row r="19" spans="1:26">
-      <c r="B19" s="61"/>
+      <c r="B19" s="67"/>
       <c r="C19">
         <v>1962</v>
       </c>
@@ -2875,7 +2877,7 @@
       </c>
     </row>
     <row r="20" spans="1:26">
-      <c r="B20" s="61"/>
+      <c r="B20" s="67"/>
       <c r="C20">
         <v>1962</v>
       </c>
@@ -2918,7 +2920,7 @@
       </c>
     </row>
     <row r="21" spans="1:26">
-      <c r="B21" s="61"/>
+      <c r="B21" s="67"/>
       <c r="C21">
         <v>1962</v>
       </c>
@@ -2961,7 +2963,7 @@
       </c>
     </row>
     <row r="22" spans="1:26">
-      <c r="B22" s="61"/>
+      <c r="B22" s="67"/>
       <c r="C22">
         <v>1962</v>
       </c>
@@ -3004,7 +3006,7 @@
       </c>
     </row>
     <row r="23" spans="1:26">
-      <c r="B23" s="61"/>
+      <c r="B23" s="67"/>
       <c r="C23">
         <v>1962</v>
       </c>
@@ -3047,7 +3049,7 @@
       </c>
     </row>
     <row r="24" spans="1:26">
-      <c r="B24" s="61"/>
+      <c r="B24" s="67"/>
       <c r="C24">
         <v>1962</v>
       </c>
@@ -3090,7 +3092,7 @@
       </c>
     </row>
     <row r="25" spans="1:26">
-      <c r="B25" s="61"/>
+      <c r="B25" s="67"/>
       <c r="C25">
         <v>1962</v>
       </c>
@@ -3133,7 +3135,7 @@
       </c>
     </row>
     <row r="26" spans="1:26">
-      <c r="B26" s="61"/>
+      <c r="B26" s="67"/>
       <c r="C26">
         <v>1962</v>
       </c>
@@ -3217,10 +3219,10 @@
       </c>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="60" t="s">
+      <c r="A28" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="61" t="s">
+      <c r="B28" s="67" t="s">
         <v>45</v>
       </c>
       <c r="C28">
@@ -3261,8 +3263,8 @@
       </c>
     </row>
     <row r="29" spans="1:26">
-      <c r="A29" s="60"/>
-      <c r="B29" s="61"/>
+      <c r="A29" s="66"/>
+      <c r="B29" s="67"/>
       <c r="C29">
         <v>1960</v>
       </c>
@@ -3301,8 +3303,8 @@
       </c>
     </row>
     <row r="30" spans="1:26">
-      <c r="A30" s="60"/>
-      <c r="B30" s="61"/>
+      <c r="A30" s="66"/>
+      <c r="B30" s="67"/>
       <c r="C30">
         <v>1960</v>
       </c>
@@ -3341,8 +3343,8 @@
       </c>
     </row>
     <row r="31" spans="1:26">
-      <c r="A31" s="60"/>
-      <c r="B31" s="61"/>
+      <c r="A31" s="66"/>
+      <c r="B31" s="67"/>
       <c r="C31">
         <v>1960</v>
       </c>
@@ -3381,8 +3383,8 @@
       </c>
     </row>
     <row r="32" spans="1:26">
-      <c r="A32" s="60"/>
-      <c r="B32" s="61"/>
+      <c r="A32" s="66"/>
+      <c r="B32" s="67"/>
       <c r="C32">
         <v>1960</v>
       </c>
@@ -3421,8 +3423,8 @@
       </c>
     </row>
     <row r="33" spans="1:26">
-      <c r="A33" s="60"/>
-      <c r="B33" s="61"/>
+      <c r="A33" s="66"/>
+      <c r="B33" s="67"/>
       <c r="C33">
         <v>1960</v>
       </c>
@@ -15743,14 +15745,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="P3:P5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="O3:O5"/>
     <mergeCell ref="A28:A33"/>
     <mergeCell ref="B28:B33"/>
     <mergeCell ref="Y3:Z3"/>
@@ -15765,6 +15759,14 @@
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="T3:V3"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="P3:P5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="O3:O5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N6" r:id="rId1" xr:uid="{C197F492-C155-453C-9706-9BEC01725253}"/>
@@ -15789,8 +15791,8 @@
   <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView zoomScale="69" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7:F85"/>
+      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="N73" sqref="N73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16"/>
@@ -15818,16 +15820,16 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1">
       <c r="A3" s="75" t="s">
@@ -15843,7 +15845,7 @@
       <c r="I3" s="75"/>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1">
-      <c r="A4" s="68"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="62" t="s">
         <v>5</v>
       </c>
@@ -15864,7 +15866,7 @@
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A5" s="68"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="62"/>
       <c r="C5" s="62"/>
       <c r="D5" s="62"/>
@@ -15874,19 +15876,19 @@
       <c r="F5" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="63" t="s">
+      <c r="G5" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="63" t="s">
+      <c r="H5" s="68" t="s">
         <v>92</v>
       </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" s="11" customFormat="1" ht="17" thickBot="1">
-      <c r="A6" s="69"/>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
       <c r="E6" s="10" t="s">
         <v>20</v>
       </c>
@@ -17088,7 +17090,7 @@
       <c r="I2" s="76"/>
     </row>
     <row r="3" spans="1:18" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="68"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="62" t="s">
         <v>5</v>
       </c>
@@ -17131,7 +17133,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="68"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
@@ -17156,10 +17158,10 @@
       <c r="Q4" s="62"/>
     </row>
     <row r="5" spans="1:18" s="17" customFormat="1" ht="18" thickBot="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -17175,9 +17177,9 @@
       <c r="I5" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
       <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
@@ -18337,17 +18339,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10">
@@ -18365,7 +18367,7 @@
       <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="68"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="62" t="s">
         <v>5</v>
       </c>
@@ -18387,26 +18389,26 @@
       <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="68"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="F4" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
       <c r="I4" s="62"/>
       <c r="J4" s="62"/>
     </row>
     <row r="5" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -18419,8 +18421,8 @@
       <c r="H5" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
     </row>
     <row r="6" spans="1:10">
       <c r="B6" s="25" t="s">
@@ -25581,7 +25583,7 @@
   <dimension ref="A1:R161"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="106" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="5" topLeftCell="A120" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F118" sqref="F118:F136"/>
     </sheetView>
   </sheetViews>
@@ -25629,7 +25631,7 @@
       <c r="I2" s="76"/>
     </row>
     <row r="3" spans="1:18" s="6" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="68"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="62" t="s">
         <v>5</v>
       </c>
@@ -25661,7 +25663,7 @@
       <c r="Q3" s="62"/>
     </row>
     <row r="4" spans="1:18" s="6" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="68"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
@@ -25691,10 +25693,10 @@
       <c r="Q4" s="62"/>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -25707,9 +25709,9 @@
       <c r="J5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
@@ -28088,6 +28090,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="A3:A5"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F3:H3"/>
@@ -28096,12 +28104,6 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -28129,17 +28131,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:11">
@@ -28157,7 +28159,7 @@
       <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="68"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="62" t="s">
         <v>5</v>
       </c>
@@ -28183,26 +28185,26 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="68"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="F4" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
       <c r="I4" s="62"/>
       <c r="J4" s="62"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -28215,8 +28217,8 @@
       <c r="H5" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
       <c r="K5" s="6" t="s">
         <v>160</v>
       </c>
@@ -31197,7 +31199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5FF47D-C774-6B45-AE66-2A4B51DD47F5}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="143" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="C6:D8"/>
     </sheetView>
@@ -31247,7 +31249,7 @@
       <c r="I2" s="76"/>
     </row>
     <row r="3" spans="1:18" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="68"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="62" t="s">
         <v>5</v>
       </c>
@@ -31274,7 +31276,7 @@
       <c r="Q3" s="62"/>
     </row>
     <row r="4" spans="1:18" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="68"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
@@ -31301,10 +31303,10 @@
       <c r="Q4" s="62"/>
     </row>
     <row r="5" spans="1:18" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -31320,9 +31322,9 @@
       <c r="I5" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
       <c r="O5" s="10"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
@@ -31712,6 +31714,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="B2:I2"/>
@@ -31719,11 +31726,6 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -31783,7 +31785,7 @@
       <c r="I2" s="76"/>
     </row>
     <row r="3" spans="1:18" s="6" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="68"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="62" t="s">
         <v>5</v>
       </c>
@@ -31806,7 +31808,7 @@
       <c r="Q3" s="62"/>
     </row>
     <row r="4" spans="1:18" s="6" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="68"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
@@ -31825,10 +31827,10 @@
       <c r="Q4" s="62"/>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -31844,9 +31846,9 @@
       <c r="I5" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
@@ -32068,17 +32070,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>